<commit_message>
[Update] IntegrationTC and CommonTC
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 3/WS_CommonTest Case_v1.0_EN .xlsx
+++ b/WIP/Documents/Report 3/WS_CommonTest Case_v1.0_EN .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="7260" tabRatio="821" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="7260" tabRatio="821" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="172">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -554,20 +554,6 @@
   </si>
   <si>
     <t>Color of all tabs selection is the same</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Dự án đã ủng hộ
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Dự án theo dõi
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
   </si>
   <si>
     <t>Message</t>
@@ -615,17 +601,6 @@
 6. Edit ID number on link to number which is not existed on list then press Enter</t>
   </si>
   <si>
-    <t>Search category</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click on category of a project
-3. Copy link
-4. Change to other browser
-5. Paste link 
-6. Edit ID number on link to number which is not existed on list then press Enter</t>
-  </si>
-  <si>
     <t>1. Login on one browser
 2. Click Tin nhắn then click on an exist mesage
 3. Copy link
@@ -712,9 +687,6 @@
     <t>Event Detail</t>
   </si>
   <si>
-    <t>Post Detail</t>
-  </si>
-  <si>
     <t>Check scroll bar</t>
   </si>
   <si>
@@ -728,13 +700,6 @@
 4. Operation System: Window 8.1 Professional 64 bit </t>
   </si>
   <si>
-    <t>1. Login on one browser
-2. Click Event đã tạo
-3. Copy link
-4. Change to other browser
-5. Paste link and press Enter</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check width of browser </t>
   </si>
   <si>
@@ -823,6 +788,58 @@
   </si>
   <si>
     <t>Display logo as design document</t>
+  </si>
+  <si>
+    <t>Searching by category</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Click on category of keywỏd
+3. Copy link
+4. Change to other browser
+5. Paste link 
+6. Edit ID number on link to number which is not existed on list then press Enter</t>
+  </si>
+  <si>
+    <t>Thread Detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Thread
+(When user doesn't login yet)
+</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Paste link: https://http://localhost:hostport/editEvent
+ and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Paste link: https://http://localhost:hostport/createThread
+ and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+Paste link: https://http://localhost:hostport/donateEvent
+ and press Enter</t>
+  </si>
+  <si>
+    <t>Created Organization
+(When user doesn't login yet)</t>
+  </si>
+  <si>
+    <t>Edit Organization
+(When user doesn't login yet)</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Paste link: https://http://localhost:hostport/createOrganization
+ and press Enter</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Paste link: https://http://localhost:hostport/editOrganization
+ and press Enter</t>
   </si>
 </sst>
 </file>
@@ -1888,6 +1905,9 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1930,9 +1950,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2413,13 +2430,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="135" t="s">
+      <c r="C2" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="135"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -2430,56 +2447,56 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="136" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="136"/>
-      <c r="E4" s="136"/>
+      <c r="C4" s="137" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="136" t="s">
-        <v>119</v>
-      </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="136"/>
+      <c r="C5" s="137" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="138" t="str">
+      <c r="C6" s="139" t="str">
         <f>C5&amp;"_"&amp;"Common Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>WS_Common Test Case_v1.0</v>
       </c>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="139"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="134" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="137"/>
-      <c r="C7" s="138"/>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="139"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="139"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2556,7 @@
         <v>54</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -2641,39 +2658,39 @@
       <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142" t="str">
+      <c r="C3" s="142"/>
+      <c r="D3" s="143" t="str">
         <f>Cover!C4</f>
         <v>WingS</v>
       </c>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="142" t="str">
+      <c r="C4" s="142"/>
+      <c r="D4" s="143" t="str">
         <f>Cover!C5</f>
         <v>WS</v>
       </c>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
     </row>
     <row r="5" spans="2:6" s="35" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="139" t="s">
+      <c r="B5" s="140" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="139"/>
-      <c r="D5" s="140" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="140"/>
-      <c r="F5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="141" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="141"/>
+      <c r="F5" s="141"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="36"/>
@@ -2851,15 +2868,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="145"/>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="145"/>
-      <c r="G1" s="145"/>
-      <c r="H1" s="145"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
+      <c r="E1" s="146"/>
+      <c r="F1" s="146"/>
+      <c r="G1" s="146"/>
+      <c r="H1" s="146"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="58"/>
@@ -2875,17 +2892,17 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="142" t="str">
+      <c r="C3" s="143" t="str">
         <f>Cover!C4</f>
         <v>WingS</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="143" t="s">
+      <c r="D3" s="143"/>
+      <c r="E3" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="143"/>
+      <c r="F3" s="144"/>
       <c r="G3" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H3" s="61"/>
     </row>
@@ -2893,17 +2910,17 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="142" t="str">
+      <c r="C4" s="143" t="str">
         <f>Cover!C5</f>
         <v>WS</v>
       </c>
-      <c r="D4" s="142"/>
-      <c r="E4" s="143" t="s">
+      <c r="D4" s="143"/>
+      <c r="E4" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="143"/>
+      <c r="F4" s="144"/>
       <c r="G4" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H4" s="61"/>
     </row>
@@ -2911,15 +2928,15 @@
       <c r="B5" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="142" t="str">
+      <c r="C5" s="143" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>WS_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="142"/>
-      <c r="E5" s="143" t="s">
+      <c r="D5" s="143"/>
+      <c r="E5" s="144" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="143"/>
+      <c r="F5" s="144"/>
       <c r="G5" s="103"/>
       <c r="H5" s="63"/>
     </row>
@@ -2928,12 +2945,12 @@
       <c r="B6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="144"/>
-      <c r="D6" s="144"/>
-      <c r="E6" s="144"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="144"/>
-      <c r="H6" s="144"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="145"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="58"/>
@@ -3459,14 +3476,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -3719,14 +3736,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -3979,14 +3996,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="147" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
+      <c r="B4" s="148" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -4246,11 +4263,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -4516,12 +4533,12 @@
         <f>COUNTIF(F11:G625,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="149">
+      <c r="E6" s="150">
         <f>COUNTA(A11:A182)*2</f>
         <v>16</v>
       </c>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -5822,13 +5839,13 @@
         <v>[User_login-2]</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="105"/>
@@ -5849,7 +5866,7 @@
         <v>63</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E13" s="106"/>
       <c r="F13" s="105"/>
@@ -5864,10 +5881,10 @@
         <v>[User_login-4]</v>
       </c>
       <c r="B14" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="105" t="s">
         <v>124</v>
-      </c>
-      <c r="C14" s="105" t="s">
-        <v>128</v>
       </c>
       <c r="D14" s="105" t="s">
         <v>64</v>
@@ -5885,13 +5902,13 @@
         <v>[User_login-5]</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E15" s="106"/>
       <c r="F15" s="105"/>
@@ -5906,13 +5923,13 @@
         <v>[User_login-6]</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E16" s="106"/>
       <c r="F16" s="105"/>
@@ -5927,13 +5944,13 @@
         <v>[User_login-7]</v>
       </c>
       <c r="B17" s="105" t="s">
+        <v>122</v>
+      </c>
+      <c r="C17" s="105" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="105" t="s">
-        <v>130</v>
-      </c>
       <c r="D17" s="105" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E17" s="106"/>
       <c r="F17" s="105"/>
@@ -5948,13 +5965,13 @@
         <v>[User_login-8]</v>
       </c>
       <c r="B18" s="105" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E18" s="106"/>
       <c r="F18" s="105"/>
@@ -5969,10 +5986,10 @@
         <v>[User_login-9]</v>
       </c>
       <c r="B19" s="105" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D19" s="105" t="s">
         <v>64</v>
@@ -6016,10 +6033,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW24"/>
+  <dimension ref="A1:IW27"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D17:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -6298,14 +6315,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="147" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -6558,14 +6575,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -6818,14 +6835,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="147" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
+      <c r="B4" s="148" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -7085,11 +7102,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -7340,11 +7357,11 @@
     </row>
     <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="113">
-        <f>COUNTIF(F11:G183,"Pass")</f>
+        <f>COUNTIF(F11:G186,"Pass")</f>
         <v>0</v>
       </c>
       <c r="B6" s="94">
-        <f>COUNTIF(F11:G630,"Fail")</f>
+        <f>COUNTIF(F11:G633,"Fail")</f>
         <v>0</v>
       </c>
       <c r="C6" s="94">
@@ -7352,15 +7369,15 @@
         <v>24</v>
       </c>
       <c r="D6" s="95">
-        <f>COUNTIF(F11:G630,"N/A")</f>
+        <f>COUNTIF(F11:G633,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="149">
-        <f>COUNTA(A11:A187)*2</f>
+      <c r="E6" s="150">
+        <f>COUNTA(A11:A190)*2</f>
         <v>24</v>
       </c>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -8660,10 +8677,10 @@
         <v>ID-2</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D12" s="105" t="s">
         <v>67</v>
@@ -8680,10 +8697,10 @@
         <v>ID-3</v>
       </c>
       <c r="B13" s="105" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>98</v>
+        <v>167</v>
       </c>
       <c r="D13" s="105" t="s">
         <v>67</v>
@@ -8699,11 +8716,11 @@
         <f>"ID-" &amp; (COUNTA(A$9:A13)+1)</f>
         <v>ID-4</v>
       </c>
-      <c r="B14" s="150" t="s">
-        <v>158</v>
+      <c r="B14" s="135" t="s">
+        <v>152</v>
       </c>
       <c r="C14" s="105" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="D14" s="105" t="s">
         <v>67</v>
@@ -8714,16 +8731,13 @@
       <c r="H14" s="105"/>
       <c r="I14" s="105"/>
     </row>
-    <row r="15" spans="1:257" s="88" customFormat="1" ht="72" customHeight="1">
-      <c r="A15" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A14)+1)</f>
-        <v>ID-5</v>
-      </c>
+    <row r="15" spans="1:257" s="88" customFormat="1" ht="75" customHeight="1">
+      <c r="A15" s="105"/>
       <c r="B15" s="105" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D15" s="105" t="s">
         <v>67</v>
@@ -8734,16 +8748,16 @@
       <c r="H15" s="105"/>
       <c r="I15" s="105"/>
     </row>
-    <row r="16" spans="1:257" s="88" customFormat="1" ht="70.5" customHeight="1">
+    <row r="16" spans="1:257" s="88" customFormat="1" ht="72" customHeight="1">
       <c r="A16" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A15)+1)</f>
-        <v>ID-6</v>
-      </c>
-      <c r="B16" s="105" t="s">
-        <v>160</v>
+        <f>"ID-" &amp; (COUNTA(A$9:A14)+1)</f>
+        <v>ID-5</v>
+      </c>
+      <c r="B16" s="135" t="s">
+        <v>164</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="D16" s="105" t="s">
         <v>67</v>
@@ -8754,16 +8768,13 @@
       <c r="H16" s="105"/>
       <c r="I16" s="105"/>
     </row>
-    <row r="17" spans="1:10" s="88" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A17" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A16)+1)</f>
-        <v>ID-7</v>
-      </c>
+    <row r="17" spans="1:10" s="88" customFormat="1" ht="72" customHeight="1">
+      <c r="A17" s="105"/>
       <c r="B17" s="105" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="D17" s="105" t="s">
         <v>67</v>
@@ -8774,16 +8785,13 @@
       <c r="H17" s="105"/>
       <c r="I17" s="105"/>
     </row>
-    <row r="18" spans="1:10" s="88" customFormat="1" ht="67.5" customHeight="1">
-      <c r="A18" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A17)+1)</f>
-        <v>ID-8</v>
-      </c>
+    <row r="18" spans="1:10" s="88" customFormat="1" ht="72" customHeight="1">
+      <c r="A18" s="105"/>
       <c r="B18" s="105" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D18" s="105" t="s">
         <v>67</v>
@@ -8794,96 +8802,93 @@
       <c r="H18" s="105"/>
       <c r="I18" s="105"/>
     </row>
-    <row r="19" spans="1:10" ht="12.75">
-      <c r="A19" s="127"/>
-      <c r="B19" s="127" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="127"/>
-      <c r="F19" s="127"/>
-      <c r="G19" s="127"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="131"/>
-      <c r="J19" s="97"/>
-    </row>
-    <row r="20" spans="1:10" ht="99" customHeight="1">
+    <row r="19" spans="1:10" s="88" customFormat="1" ht="70.5" customHeight="1">
+      <c r="A19" s="105" t="str">
+        <f>"ID-" &amp; (COUNTA(A$9:A16)+1)</f>
+        <v>ID-6</v>
+      </c>
+      <c r="B19" s="105" t="s">
+        <v>154</v>
+      </c>
+      <c r="C19" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="105"/>
+      <c r="I19" s="105"/>
+    </row>
+    <row r="20" spans="1:10" s="88" customFormat="1" ht="70.5" customHeight="1">
       <c r="A20" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A19)+1)</f>
-        <v>ID-9</v>
+        <v>ID-7</v>
       </c>
       <c r="B20" s="105" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="C20" s="105" t="s">
-        <v>106</v>
+        <v>156</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="E20" s="105"/>
       <c r="F20" s="105"/>
       <c r="G20" s="105"/>
       <c r="H20" s="105"/>
       <c r="I20" s="105"/>
-      <c r="J20" s="97"/>
-    </row>
-    <row r="21" spans="1:10" ht="99" customHeight="1">
+    </row>
+    <row r="21" spans="1:10" s="88" customFormat="1" ht="67.5" customHeight="1">
       <c r="A21" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A20)+1)</f>
-        <v>ID-10</v>
+        <v>ID-8</v>
       </c>
       <c r="B21" s="105" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="C21" s="105" t="s">
-        <v>106</v>
+        <v>158</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="E21" s="105"/>
       <c r="F21" s="105"/>
       <c r="G21" s="105"/>
       <c r="H21" s="105"/>
       <c r="I21" s="105"/>
-      <c r="J21" s="97"/>
-    </row>
-    <row r="22" spans="1:10" ht="114.75" customHeight="1">
-      <c r="A22" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A21)+1)</f>
-        <v>ID-11</v>
-      </c>
-      <c r="B22" s="105" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="105" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="105" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="105"/>
-      <c r="I22" s="105"/>
+    </row>
+    <row r="22" spans="1:10" ht="12.75">
+      <c r="A22" s="127"/>
+      <c r="B22" s="127" t="s">
+        <v>103</v>
+      </c>
+      <c r="C22" s="127"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="131"/>
       <c r="J22" s="97"/>
     </row>
-    <row r="23" spans="1:10" ht="103.5" customHeight="1">
+    <row r="23" spans="1:10" ht="99" customHeight="1">
       <c r="A23" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A22)+1)</f>
-        <v>ID-12</v>
+        <v>ID-9</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>110</v>
+        <v>134</v>
       </c>
       <c r="C23" s="105" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E23" s="105"/>
       <c r="F23" s="105"/>
@@ -8892,19 +8897,19 @@
       <c r="I23" s="105"/>
       <c r="J23" s="97"/>
     </row>
-    <row r="24" spans="1:10" ht="114" customHeight="1">
+    <row r="24" spans="1:10" ht="99" customHeight="1">
       <c r="A24" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A23)+1)</f>
-        <v>ID-13</v>
+        <v>ID-10</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="C24" s="105" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E24" s="105"/>
       <c r="F24" s="105"/>
@@ -8912,6 +8917,69 @@
       <c r="H24" s="105"/>
       <c r="I24" s="105"/>
       <c r="J24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" ht="114.75" customHeight="1">
+      <c r="A25" s="105" t="str">
+        <f>"ID-" &amp; (COUNTA(A$9:A24)+1)</f>
+        <v>ID-11</v>
+      </c>
+      <c r="B25" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="105" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105"/>
+      <c r="H25" s="105"/>
+      <c r="I25" s="105"/>
+      <c r="J25" s="97"/>
+    </row>
+    <row r="26" spans="1:10" ht="103.5" customHeight="1">
+      <c r="A26" s="105" t="str">
+        <f>"ID-" &amp; (COUNTA(A$9:A25)+1)</f>
+        <v>ID-12</v>
+      </c>
+      <c r="B26" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="105"/>
+      <c r="F26" s="105"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105"/>
+      <c r="I26" s="105"/>
+      <c r="J26" s="97"/>
+    </row>
+    <row r="27" spans="1:10" ht="114" customHeight="1">
+      <c r="A27" s="105" t="str">
+        <f>"ID-" &amp; (COUNTA(A$9:A26)+1)</f>
+        <v>ID-13</v>
+      </c>
+      <c r="B27" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="97"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -8927,13 +8995,13 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IU12:JB18 SQ12:SX18 ACM12:ACT18 AMI12:AMP18 AWE12:AWL18 BGA12:BGH18 BPW12:BQD18 BZS12:BZZ18 CJO12:CJV18 CTK12:CTR18 DDG12:DDN18 DNC12:DNJ18 DWY12:DXF18 EGU12:EHB18 EQQ12:EQX18 FAM12:FAT18 FKI12:FKP18 FUE12:FUL18 GEA12:GEH18 GNW12:GOD18 GXS12:GXZ18 HHO12:HHV18 HRK12:HRR18 IBG12:IBN18 ILC12:ILJ18 IUY12:IVF18 JEU12:JFB18 JOQ12:JOX18 JYM12:JYT18 KII12:KIP18 KSE12:KSL18 LCA12:LCH18 LLW12:LMD18 LVS12:LVZ18 MFO12:MFV18 MPK12:MPR18 MZG12:MZN18 NJC12:NJJ18 NSY12:NTF18 OCU12:ODB18 OMQ12:OMX18 OWM12:OWT18 PGI12:PGP18 PQE12:PQL18 QAA12:QAH18 QJW12:QKD18 QTS12:QTZ18 RDO12:RDV18 RNK12:RNR18 RXG12:RXN18 SHC12:SHJ18 SQY12:SRF18 TAU12:TBB18 TKQ12:TKX18 TUM12:TUT18 UEI12:UEP18 UOE12:UOL18 UYA12:UYH18 VHW12:VID18 VRS12:VRZ18 WBO12:WBV18 WLK12:WLR18 WVG12:WVN18 WLU11:WLU23 VSC11:VSC23 WVQ11:WVQ23 WBY11:WBY23 WVG20:WVN23 WLK20:WLR23 WBO20:WBV23 VRS20:VRZ23 VHW20:VID23 UYA20:UYH23 UOE20:UOL23 UEI20:UEP23 TUM20:TUT23 TKQ20:TKX23 TAU20:TBB23 SQY20:SRF23 SHC20:SHJ23 RXG20:RXN23 RNK20:RNR23 RDO20:RDV23 QTS20:QTZ23 QJW20:QKD23 QAA20:QAH23 PQE20:PQL23 PGI20:PGP23 OWM20:OWT23 OMQ20:OMX23 OCU20:ODB23 NSY20:NTF23 NJC20:NJJ23 MZG20:MZN23 MPK20:MPR23 MFO20:MFV23 LVS20:LVZ23 LLW20:LMD23 LCA20:LCH23 KSE20:KSL23 KII20:KIP23 JYM20:JYT23 JOQ20:JOX23 JEU20:JFB23 IUY20:IVF23 ILC20:ILJ23 IBG20:IBN23 HRK20:HRR23 HHO20:HHV23 GXS20:GXZ23 GNW20:GOD23 GEA20:GEH23 FUE20:FUL23 FKI20:FKP23 FAM20:FAT23 EQQ20:EQX23 EGU20:EHB23 DWY20:DXF23 DNC20:DNJ23 DDG20:DDN23 CTK20:CTR23 CJO20:CJV23 BZS20:BZZ23 BPW20:BQD23 BGA20:BGH23 AWE20:AWL23 AMI20:AMP23 ACM20:ACT23 SQ20:SX23 IU20:JB23 JE11:JE23 TA11:TA23 ACW11:ACW23 AMS11:AMS23 AWO11:AWO23 BGK11:BGK23 BQG11:BQG23 CAC11:CAC23 CJY11:CJY23 CTU11:CTU23 DDQ11:DDQ23 DNM11:DNM23 DXI11:DXI23 EHE11:EHE23 ERA11:ERA23 FAW11:FAW23 FKS11:FKS23 FUO11:FUO23 GEK11:GEK23 GOG11:GOG23 GYC11:GYC23 HHY11:HHY23 HRU11:HRU23 IBQ11:IBQ23 ILM11:ILM23 IVI11:IVI23 JFE11:JFE23 JPA11:JPA23 JYW11:JYW23 KIS11:KIS23 KSO11:KSO23 LCK11:LCK23 LMG11:LMG23 LWC11:LWC23 MFY11:MFY23 MPU11:MPU23 MZQ11:MZQ23 NJM11:NJM23 NTI11:NTI23 ODE11:ODE23 ONA11:ONA23 OWW11:OWW23 PGS11:PGS23 PQO11:PQO23 QAK11:QAK23 QKG11:QKG23 QUC11:QUC23 RDY11:RDY23 RNU11:RNU23 RXQ11:RXQ23 SHM11:SHM23 SRI11:SRI23 TBE11:TBE23 TLA11:TLA23 TUW11:TUW23 UES11:UES23 UOO11:UOO23 UYK11:UYK23 VIG11:VIG23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IU12:JB21 SQ12:SX21 ACM12:ACT21 AMI12:AMP21 AWE12:AWL21 BGA12:BGH21 BPW12:BQD21 BZS12:BZZ21 CJO12:CJV21 CTK12:CTR21 DDG12:DDN21 DNC12:DNJ21 DWY12:DXF21 EGU12:EHB21 EQQ12:EQX21 FAM12:FAT21 FKI12:FKP21 FUE12:FUL21 GEA12:GEH21 GNW12:GOD21 GXS12:GXZ21 HHO12:HHV21 HRK12:HRR21 IBG12:IBN21 ILC12:ILJ21 IUY12:IVF21 JEU12:JFB21 JOQ12:JOX21 JYM12:JYT21 KII12:KIP21 KSE12:KSL21 LCA12:LCH21 LLW12:LMD21 LVS12:LVZ21 MFO12:MFV21 MPK12:MPR21 MZG12:MZN21 NJC12:NJJ21 NSY12:NTF21 OCU12:ODB21 OMQ12:OMX21 OWM12:OWT21 PGI12:PGP21 PQE12:PQL21 QAA12:QAH21 QJW12:QKD21 QTS12:QTZ21 RDO12:RDV21 RNK12:RNR21 RXG12:RXN21 SHC12:SHJ21 SQY12:SRF21 TAU12:TBB21 TKQ12:TKX21 TUM12:TUT21 UEI12:UEP21 UOE12:UOL21 UYA12:UYH21 VHW12:VID21 VRS12:VRZ21 WBO12:WBV21 WLK12:WLR21 WVG12:WVN21 WLU11:WLU26 VSC11:VSC26 WVQ11:WVQ26 WBY11:WBY26 WVG23:WVN26 WLK23:WLR26 WBO23:WBV26 VRS23:VRZ26 VHW23:VID26 UYA23:UYH26 UOE23:UOL26 UEI23:UEP26 TUM23:TUT26 TKQ23:TKX26 TAU23:TBB26 SQY23:SRF26 SHC23:SHJ26 RXG23:RXN26 RNK23:RNR26 RDO23:RDV26 QTS23:QTZ26 QJW23:QKD26 QAA23:QAH26 PQE23:PQL26 PGI23:PGP26 OWM23:OWT26 OMQ23:OMX26 OCU23:ODB26 NSY23:NTF26 NJC23:NJJ26 MZG23:MZN26 MPK23:MPR26 MFO23:MFV26 LVS23:LVZ26 LLW23:LMD26 LCA23:LCH26 KSE23:KSL26 KII23:KIP26 JYM23:JYT26 JOQ23:JOX26 JEU23:JFB26 IUY23:IVF26 ILC23:ILJ26 IBG23:IBN26 HRK23:HRR26 HHO23:HHV26 GXS23:GXZ26 GNW23:GOD26 GEA23:GEH26 FUE23:FUL26 FKI23:FKP26 FAM23:FAT26 EQQ23:EQX26 EGU23:EHB26 DWY23:DXF26 DNC23:DNJ26 DDG23:DDN26 CTK23:CTR26 CJO23:CJV26 BZS23:BZZ26 BPW23:BQD26 BGA23:BGH26 AWE23:AWL26 AMI23:AMP26 ACM23:ACT26 SQ23:SX26 IU23:JB26 JE11:JE26 TA11:TA26 ACW11:ACW26 AMS11:AMS26 AWO11:AWO26 BGK11:BGK26 BQG11:BQG26 CAC11:CAC26 CJY11:CJY26 CTU11:CTU26 DDQ11:DDQ26 DNM11:DNM26 DXI11:DXI26 EHE11:EHE26 ERA11:ERA26 FAW11:FAW26 FKS11:FKS26 FUO11:FUO26 GEK11:GEK26 GOG11:GOG26 GYC11:GYC26 HHY11:HHY26 HRU11:HRU26 IBQ11:IBQ26 ILM11:ILM26 IVI11:IVI26 JFE11:JFE26 JPA11:JPA26 JYW11:JYW26 KIS11:KIS26 KSO11:KSO26 LCK11:LCK26 LMG11:LMG26 LWC11:LWC26 MFY11:MFY26 MPU11:MPU26 MZQ11:MZQ26 NJM11:NJM26 NTI11:NTI26 ODE11:ODE26 ONA11:ONA26 OWW11:OWW26 PGS11:PGS26 PQO11:PQO26 QAK11:QAK26 QKG11:QKG26 QUC11:QUC26 RDY11:RDY26 RNU11:RNU26 RXQ11:RXQ26 SHM11:SHM26 SRI11:SRI26 TBE11:TBE26 TLA11:TLA26 TUW11:TUW26 UES11:UES26 UOO11:UOO26 UYK11:UYK26 VIG11:VIG26">
       <formula1>"OK,NG,N/A"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G25:G65255">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G28:G65258">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F20:G24 F12:G18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:G27 F12:G21">
       <formula1>$A$5:$D$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -8950,7 +9018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -9230,14 +9298,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="146" t="s">
+      <c r="B2" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="147"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="147"/>
+      <c r="G2" s="147"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -9490,14 +9558,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="146" t="s">
+      <c r="B3" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="146"/>
-      <c r="D3" s="146"/>
-      <c r="E3" s="146"/>
-      <c r="F3" s="146"/>
-      <c r="G3" s="146"/>
+      <c r="C3" s="147"/>
+      <c r="D3" s="147"/>
+      <c r="E3" s="147"/>
+      <c r="F3" s="147"/>
+      <c r="G3" s="147"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -9750,14 +9818,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="147" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="147"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="147"/>
-      <c r="G4" s="147"/>
+      <c r="B4" s="148" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
+      <c r="F4" s="148"/>
+      <c r="G4" s="148"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -10017,11 +10085,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="148" t="s">
+      <c r="E5" s="149" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -10287,12 +10355,12 @@
         <f>COUNTIF(F11:G633,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="149">
+      <c r="E6" s="150">
         <f>COUNTA(A11:A190)*2</f>
         <v>32</v>
       </c>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
+      <c r="F6" s="150"/>
+      <c r="G6" s="150"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -11591,13 +11659,13 @@
         <v>ID-2</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C12" s="105" t="s">
         <v>69</v>
       </c>
       <c r="D12" s="133" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E12" s="105"/>
       <c r="F12" s="105"/>
@@ -11611,13 +11679,13 @@
         <v>ID-2</v>
       </c>
       <c r="B13" s="105" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="E13" s="105"/>
       <c r="F13" s="105"/>
@@ -11631,13 +11699,13 @@
         <v>ID-3</v>
       </c>
       <c r="B14" s="105" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C14" s="105" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E14" s="105"/>
       <c r="F14" s="105"/>
@@ -11651,13 +11719,13 @@
         <v>ID-4</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E15" s="105"/>
       <c r="F15" s="105"/>
@@ -11671,13 +11739,13 @@
         <v>ID-5</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E16" s="105"/>
       <c r="F16" s="105"/>
@@ -11697,7 +11765,7 @@
         <v>71</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E17" s="105"/>
       <c r="F17" s="105"/>
@@ -11737,7 +11805,7 @@
         <v>76</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E19" s="105"/>
       <c r="F19" s="105"/>
@@ -11871,13 +11939,13 @@
         <v>ID-16</v>
       </c>
       <c r="B26" s="105" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C26" s="105" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E26" s="105"/>
       <c r="F26" s="105"/>

</xml_diff>

<commit_message>
[Add] Checklist TC [Update] Common TC
</commit_message>
<xml_diff>
--- a/WIP/Documents/Report 3/WS_CommonTest Case_v1.0_EN .xlsx
+++ b/WIP/Documents/Report 3/WS_CommonTest Case_v1.0_EN .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="7260" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19110" windowHeight="7260" tabRatio="821" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test case List" sheetId="2" r:id="rId1"/>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="190">
   <si>
     <t>TEST CASE</t>
   </si>
@@ -403,9 +403,6 @@
     <t>Back to Test Report</t>
   </si>
   <si>
-    <t>User_login</t>
-  </si>
-  <si>
     <t>This test cases were created to test integration between login with all functions and all functions together</t>
   </si>
   <si>
@@ -418,10 +415,6 @@
     <t>Check order of pointer when enter Tab</t>
   </si>
   <si>
-    <t>1. Go to the page have field need to fill in (Login, register, Create Project, Update Project, ...)
-2. From one text field, enter Tab</t>
-  </si>
-  <si>
     <t>1. Go to Homepage</t>
   </si>
   <si>
@@ -440,13 +433,6 @@
     <t>Check width of page</t>
   </si>
   <si>
-    <t>Check display greeting when user login successfully</t>
-  </si>
-  <si>
-    <t>1. Login successfully
-2. Confirm display greeting</t>
-  </si>
-  <si>
     <t>Check header of screen</t>
   </si>
   <si>
@@ -504,9 +490,6 @@
     <t>Mouse hover over link</t>
   </si>
   <si>
-    <t>Mouse pointer has hand symbol</t>
-  </si>
-  <si>
     <t>Check tab selection color</t>
   </si>
   <si>
@@ -523,9 +506,6 @@
   </si>
   <si>
     <t>Color of all tabs selection is the same</t>
-  </si>
-  <si>
-    <t>Message</t>
   </si>
   <si>
     <t>1. Login on one browser
@@ -548,33 +528,7 @@
     <t>Edit ID on link</t>
   </si>
   <si>
-    <t>1. Login on one browser
-2. Click on one exist project
-3. Copy link
-4. Change to other browser
-5. Paste link 
-6. Edit ID number on link to number which is not existed on list then press Enter</t>
-  </si>
-  <si>
     <t>Return to Error page</t>
-  </si>
-  <si>
-    <t>Public profile</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click on one exist project then click on Creator
-3. Copy link
-4. Change to other browser
-5. Paste link 
-6. Edit ID number on link to number which is not existed on list then press Enter</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click Tin nhắn then click on an exist mesage
-3. Copy link
-5. Paste link 
-6. Edit ID number on link to number which is not existed on list then press Enter</t>
   </si>
   <si>
     <t>1. Open web page
@@ -602,12 +556,6 @@
     <t>WS_CommonTest Case_v1.0_EN</t>
   </si>
   <si>
-    <t>Check click on 'WingS'</t>
-  </si>
-  <si>
-    <t>Click on 'WingS'</t>
-  </si>
-  <si>
     <t>Check click on 'Sự kiện'</t>
   </si>
   <si>
@@ -620,22 +568,13 @@
     <t>Check click on 'Về chúng tôi'</t>
   </si>
   <si>
-    <t>Check click on 'Lên hệ'</t>
-  </si>
-  <si>
     <t>click on 'Trang chủ'</t>
   </si>
   <si>
-    <t>Click on 'Lên hệ'</t>
-  </si>
-  <si>
     <t>Click on 'Về chúng tôi'</t>
   </si>
   <si>
     <t>Click on 'Sự kiện'</t>
-  </si>
-  <si>
-    <t>1. Go to Contact page</t>
   </si>
   <si>
     <t>Click on 'Thảo luận'</t>
@@ -667,17 +606,6 @@
   <si>
     <t>- Width of page is full
 - Scrollbar of browser is displayed</t>
-  </si>
-  <si>
-    <t>1. Homepage is displayed 
-2. Display Contact page</t>
-  </si>
-  <si>
-    <t>When clicking on link at Home page screen</t>
-  </si>
-  <si>
-    <t>1. Go to Home page  
-2. Click on Liên hệ at footer</t>
   </si>
   <si>
     <t>--/--/2016</t>
@@ -752,17 +680,6 @@
     <t>Display logo as design document</t>
   </si>
   <si>
-    <t>Searching by category</t>
-  </si>
-  <si>
-    <t>1. Login on one browser
-2. Click on category of keywỏd
-3. Copy link
-4. Change to other browser
-5. Paste link 
-6. Edit ID number on link to number which is not existed on list then press Enter</t>
-  </si>
-  <si>
     <t>Thread Detail</t>
   </si>
   <si>
@@ -824,6 +741,141 @@
 2. Database server: SQL Server 2012
 3. Browser: Google Chrome 53, Mozzila Firefox 50
 4. Operation System: Window 8.1 Professional 64 bit </t>
+  </si>
+  <si>
+    <t>1. Go to the page have field need to fill in (Logo, Homepage, Event, Thread, Organization ...)
+2. From one text field, enter Tab</t>
+  </si>
+  <si>
+    <t>Check click on 'Tìm kiếm'</t>
+  </si>
+  <si>
+    <t>Click on 'Tìm kiếm''</t>
+  </si>
+  <si>
+    <t>1. Go to Searching page</t>
+  </si>
+  <si>
+    <t>Check click on 'Tổ chức'</t>
+  </si>
+  <si>
+    <t>Click on 'Tổ chức'</t>
+  </si>
+  <si>
+    <t>1.Go to Organization page</t>
+  </si>
+  <si>
+    <t>Check click on Logo page</t>
+  </si>
+  <si>
+    <t>click on Logo</t>
+  </si>
+  <si>
+    <t>Check click on 'Facebook' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Facebook' on footer</t>
+  </si>
+  <si>
+    <t>1. Go to link Facebook of WS</t>
+  </si>
+  <si>
+    <t>Check click on 'Google' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Twitter' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Trang chủ' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Sự kiện' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Tổ chức' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Thảo luận' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Về chúng tôi' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Liên hệ' on footer</t>
+  </si>
+  <si>
+    <t>Check click on 'Đăng nhập' on footer</t>
+  </si>
+  <si>
+    <t>Click on 'Đăng nhập' on footer</t>
+  </si>
+  <si>
+    <t>Click on 'Liên hệ' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Về chúng tôi' on footer</t>
+  </si>
+  <si>
+    <t>Click on 'Thảo luận' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Tổ chức' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Sự kiện' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Trang chủ' on footer</t>
+  </si>
+  <si>
+    <t>Click on  'Twitter' on footer</t>
+  </si>
+  <si>
+    <t>Click on 'Google' on footer</t>
+  </si>
+  <si>
+    <t>1. Go to link Google link of WS</t>
+  </si>
+  <si>
+    <t>1. Go to link Twitter of WS</t>
+  </si>
+  <si>
+    <t>1.Go to Contact page</t>
+  </si>
+  <si>
+    <t>1.Go to Login page</t>
+  </si>
+  <si>
+    <t>Check display avatar when user login successfully</t>
+  </si>
+  <si>
+    <t>1. Login successfully
+2. Confirm display avatar</t>
+  </si>
+  <si>
+    <t>Focus tab when move mouse to these tab</t>
+  </si>
+  <si>
+    <t>User profile</t>
+  </si>
+  <si>
+    <t>Organization Detail</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Enter link in URL: …/Profile/Duytn345345</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. …/Organizationdetail/9999</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Enter link in URL: …/Threaddetail/99999</t>
+  </si>
+  <si>
+    <t>1. Login on one browser
+2. Go URL: ../eventdetail/99999</t>
   </si>
 </sst>
 </file>
@@ -1534,7 +1586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1892,6 +1944,22 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1903,16 +1971,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1934,9 +1992,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2398,7 +2453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
@@ -2426,39 +2481,39 @@
       <c r="E2" s="34"/>
     </row>
     <row r="3" spans="2:6">
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="140" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143" t="str">
+      <c r="C3" s="140"/>
+      <c r="D3" s="141" t="str">
         <f>Cover!C4</f>
         <v>WingS</v>
       </c>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="140" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="142"/>
-      <c r="D4" s="143" t="str">
+      <c r="C4" s="140"/>
+      <c r="D4" s="141" t="str">
         <f>Cover!C5</f>
         <v>WS</v>
       </c>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="141"/>
     </row>
     <row r="5" spans="2:6" s="35" customFormat="1" ht="72" customHeight="1">
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="141" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" s="141"/>
-      <c r="F5" s="141"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="139" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="139"/>
+      <c r="F5" s="139"/>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="36"/>
@@ -2496,13 +2551,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="151" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="D9" s="136" t="s">
+        <v>50</v>
       </c>
       <c r="E9" s="102" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="F9" s="101"/>
     </row>
@@ -2511,13 +2566,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="151" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="D10" s="136" t="s">
+        <v>53</v>
       </c>
       <c r="E10" s="102" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="F10" s="101"/>
     </row>
@@ -2526,13 +2581,13 @@
         <v>3</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="151" t="s">
-        <v>58</v>
+        <v>56</v>
+      </c>
+      <c r="D11" s="136" t="s">
+        <v>56</v>
       </c>
       <c r="E11" s="102" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="F11" s="49"/>
     </row>
@@ -2627,7 +2682,7 @@
   <dimension ref="A2:G18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2645,13 +2700,13 @@
     <row r="2" spans="1:7" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="136" t="s">
+      <c r="C2" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="136"/>
-      <c r="E2" s="136"/>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" s="6"/>
@@ -2662,56 +2717,56 @@
       <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="137" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="137"/>
-      <c r="E4" s="137"/>
+      <c r="C4" s="143" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
       <c r="F4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="137" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="137"/>
-      <c r="E5" s="137"/>
+      <c r="C5" s="143" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="143"/>
+      <c r="E5" s="143"/>
       <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="144" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="139" t="str">
+      <c r="C6" s="145" t="str">
         <f>C5&amp;"_"&amp;"Common Test Case"&amp;"_"&amp;"v1.0"</f>
         <v>WS_Common Test Case_v1.0</v>
       </c>
-      <c r="D6" s="139"/>
-      <c r="E6" s="139"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
       <c r="F6" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="134" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="13.5" customHeight="1">
-      <c r="B7" s="138"/>
-      <c r="C7" s="139"/>
-      <c r="D7" s="139"/>
-      <c r="E7" s="139"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="145"/>
+      <c r="D7" s="145"/>
+      <c r="E7" s="145"/>
       <c r="F7" s="9" t="s">
         <v>7</v>
       </c>
@@ -2768,10 +2823,10 @@
         <v>46</v>
       </c>
       <c r="F12" s="104" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="19" customFormat="1" ht="21.75" customHeight="1">
@@ -2846,7 +2901,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2860,15 +2915,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" customHeight="1">
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="148" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
+      <c r="C1" s="148"/>
+      <c r="D1" s="148"/>
+      <c r="E1" s="148"/>
+      <c r="F1" s="148"/>
+      <c r="G1" s="148"/>
+      <c r="H1" s="148"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
       <c r="A2" s="58"/>
@@ -2884,17 +2939,17 @@
       <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="143" t="str">
+      <c r="C3" s="141" t="str">
         <f>Cover!C4</f>
         <v>WingS</v>
       </c>
-      <c r="D3" s="143"/>
-      <c r="E3" s="144" t="s">
+      <c r="D3" s="141"/>
+      <c r="E3" s="146" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="144"/>
+      <c r="F3" s="146"/>
       <c r="G3" s="10" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H3" s="61"/>
     </row>
@@ -2902,17 +2957,17 @@
       <c r="B4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="143" t="str">
+      <c r="C4" s="141" t="str">
         <f>Cover!C5</f>
         <v>WS</v>
       </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="144" t="s">
+      <c r="D4" s="141"/>
+      <c r="E4" s="146" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="144"/>
+      <c r="F4" s="146"/>
       <c r="G4" s="10" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H4" s="61"/>
     </row>
@@ -2920,15 +2975,15 @@
       <c r="B5" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="143" t="str">
+      <c r="C5" s="141" t="str">
         <f>C4&amp;"_"&amp;"Integration Test Report"&amp;"_"&amp;"v1.0"</f>
         <v>WS_Integration Test Report_v1.0</v>
       </c>
-      <c r="D5" s="143"/>
-      <c r="E5" s="144" t="s">
+      <c r="D5" s="141"/>
+      <c r="E5" s="146" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="144"/>
+      <c r="F5" s="146"/>
       <c r="G5" s="103"/>
       <c r="H5" s="63"/>
     </row>
@@ -2937,12 +2992,12 @@
       <c r="B6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="145"/>
-      <c r="D6" s="145"/>
-      <c r="E6" s="145"/>
-      <c r="F6" s="145"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="145"/>
+      <c r="C6" s="147"/>
+      <c r="D6" s="147"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
+      <c r="H6" s="147"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="A7" s="58"/>
@@ -3003,19 +3058,19 @@
         <v>1</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="72">
         <f>Common!A6</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E11" s="72">
         <f>Common!B6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="72">
         <f>Common!C6</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G11" s="72">
         <f>Common!D6</f>
@@ -3023,7 +3078,7 @@
       </c>
       <c r="H11" s="73">
         <f>Common!E6</f>
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3032,19 +3087,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="119" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="72">
         <f>Security!A6</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E12" s="72">
         <f>Security!B6</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F12" s="72">
         <f>Security!C6</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G12" s="72">
         <f>Security!D6</f>
@@ -3052,7 +3107,7 @@
       </c>
       <c r="H12" s="73">
         <f>Security!E6</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3061,11 +3116,11 @@
         <v>3</v>
       </c>
       <c r="C13" s="119" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="72">
         <f>UI!A6</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E13" s="72">
         <f>UI!B6</f>
@@ -3073,7 +3128,7 @@
       </c>
       <c r="F13" s="72">
         <f>UI!C6</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G13" s="72">
         <f>UI!D6</f>
@@ -3092,15 +3147,15 @@
       </c>
       <c r="D14" s="75">
         <f>SUM(D11:D13)</f>
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="E14" s="75">
         <f t="shared" ref="E14:H14" si="0">SUM(E11:E13)</f>
+        <v>28</v>
+      </c>
+      <c r="F14" s="75">
+        <f>SUM(F11:F13)</f>
         <v>0</v>
-      </c>
-      <c r="F14" s="75">
-        <f t="shared" si="0"/>
-        <v>72</v>
       </c>
       <c r="G14" s="75">
         <f t="shared" si="0"/>
@@ -3108,7 +3163,7 @@
       </c>
       <c r="H14" s="75">
         <f t="shared" si="0"/>
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3130,7 +3185,7 @@
       <c r="D16" s="66"/>
       <c r="E16" s="80">
         <f>(D14+E14)*100/(H14-G14)</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F16" s="66" t="s">
         <v>43</v>
@@ -3147,7 +3202,7 @@
       <c r="D17" s="66"/>
       <c r="E17" s="80">
         <f>D14*100/(H14-G14)</f>
-        <v>0</v>
+        <v>70.833333333333329</v>
       </c>
       <c r="F17" s="66" t="s">
         <v>43</v>
@@ -3186,10 +3241,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IW19"/>
+  <dimension ref="A1:IW29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -3468,14 +3523,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="147" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="B2" s="149" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -3728,14 +3783,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="147" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
+      <c r="B3" s="149" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -3988,14 +4043,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="148" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
+      <c r="B4" s="150" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -4255,11 +4310,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -4510,27 +4565,27 @@
     </row>
     <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="113">
-        <f>COUNTIF(F11:G178,"Pass")</f>
-        <v>0</v>
+        <f>COUNTIF(F11:G177,"Pass")</f>
+        <v>34</v>
       </c>
       <c r="B6" s="94">
-        <f>COUNTIF(F11:G625,"Fail")</f>
-        <v>0</v>
+        <f>COUNTIF(F11:G624,"Fail")</f>
+        <v>2</v>
       </c>
       <c r="C6" s="94">
         <f>E6-D6-B6-A6</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D6" s="95">
-        <f>COUNTIF(F11:G625,"N/A")</f>
+        <f>COUNTIF(F11:G624,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="150">
-        <f>COUNTA(A11:A182)*2</f>
-        <v>16</v>
-      </c>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
+      <c r="E6" s="152">
+        <f>COUNTA(A11:A181)*2</f>
+        <v>36</v>
+      </c>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -5557,10 +5612,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>35</v>
@@ -5814,7 +5869,7 @@
     <row r="11" spans="1:257" ht="14.25" customHeight="1">
       <c r="A11" s="127"/>
       <c r="B11" s="127" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="125"/>
       <c r="D11" s="125"/>
@@ -5825,173 +5880,491 @@
       <c r="I11" s="126"/>
       <c r="J11" s="97"/>
     </row>
-    <row r="12" spans="1:257" ht="28.5" customHeight="1">
+    <row r="12" spans="1:257" ht="14.25" customHeight="1">
       <c r="A12" s="124" t="str">
-        <f>IF(OR(B12&lt;&gt;"",D12&lt;E11&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-2]</v>
+        <f t="shared" ref="A12:A17" si="0">IF(OR(B12&lt;&gt;"",D12&lt;E11&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-2]</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>130</v>
+        <v>51</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="E12" s="106"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="107"/>
+      <c r="F12" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="107">
+        <v>42684</v>
+      </c>
       <c r="I12" s="108"/>
       <c r="J12" s="97"/>
     </row>
-    <row r="13" spans="1:257" ht="12" customHeight="1">
+    <row r="13" spans="1:257" ht="13.5" customHeight="1">
       <c r="A13" s="124" t="str">
-        <f t="shared" ref="A13:A15" si="0">IF(OR(B13&lt;&gt;"",D13&lt;E12&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-3]</v>
+        <f t="shared" si="0"/>
+        <v>[Common-3]</v>
       </c>
       <c r="B13" s="105" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="105" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="105" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="105" t="s">
-        <v>92</v>
-      </c>
       <c r="E13" s="106"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="107"/>
+      <c r="F13" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="107">
+        <v>42684</v>
+      </c>
       <c r="I13" s="108"/>
       <c r="J13" s="97"/>
     </row>
-    <row r="14" spans="1:257" ht="18" customHeight="1">
+    <row r="14" spans="1:257" ht="12.75" customHeight="1">
       <c r="A14" s="124" t="str">
         <f t="shared" si="0"/>
-        <v>[User_login-4]</v>
+        <v>[Common-4]</v>
       </c>
       <c r="B14" s="105" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C14" s="105" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="106"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="107"/>
+      <c r="F14" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="107">
+        <v>42684</v>
+      </c>
       <c r="I14" s="108"/>
       <c r="J14" s="97"/>
     </row>
-    <row r="15" spans="1:257" ht="19.5" customHeight="1">
+    <row r="15" spans="1:257" ht="14.25" customHeight="1">
       <c r="A15" s="124" t="str">
         <f t="shared" si="0"/>
-        <v>[User_login-5]</v>
+        <v>[Common-5]</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E15" s="106"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="107"/>
+      <c r="F15" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="107">
+        <v>42684</v>
+      </c>
       <c r="I15" s="108"/>
       <c r="J15" s="97"/>
     </row>
     <row r="16" spans="1:257" ht="14.25" customHeight="1">
       <c r="A16" s="124" t="str">
-        <f>IF(OR(B16&lt;&gt;"",D16&lt;E11&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-6]</v>
+        <f t="shared" si="0"/>
+        <v>[Common-6]</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E16" s="106"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="107"/>
+      <c r="F16" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="107">
+        <v>42684</v>
+      </c>
       <c r="I16" s="108"/>
       <c r="J16" s="97"/>
     </row>
     <row r="17" spans="1:10" ht="14.25" customHeight="1">
       <c r="A17" s="124" t="str">
-        <f>IF(OR(B17&lt;&gt;"",D17&lt;E12&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-7]</v>
+        <f t="shared" si="0"/>
+        <v>[Common-7]</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
       <c r="E17" s="106"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="107"/>
+      <c r="F17" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="107">
+        <v>42684</v>
+      </c>
       <c r="I17" s="108"/>
       <c r="J17" s="97"/>
     </row>
     <row r="18" spans="1:10" ht="14.25" customHeight="1">
       <c r="A18" s="124" t="str">
-        <f>IF(OR(B18&lt;&gt;"",D18&lt;E13&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-8]</v>
+        <f>IF(OR(B18&lt;&gt;"",D18&lt;E12&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-8]</v>
       </c>
       <c r="B18" s="105" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="E18" s="106"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="107"/>
+      <c r="F18" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="107">
+        <v>42684</v>
+      </c>
       <c r="I18" s="108"/>
       <c r="J18" s="97"/>
     </row>
-    <row r="19" spans="1:10" ht="14.25" customHeight="1">
+    <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="124" t="str">
-        <f>IF(OR(B19&lt;&gt;"",D19&lt;E14&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
-        <v>[User_login-9]</v>
+        <f>IF(OR(B19&lt;&gt;"",D19&lt;E13&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-9]</v>
       </c>
       <c r="B19" s="105" t="s">
-        <v>107</v>
+        <v>148</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>54</v>
+        <v>150</v>
       </c>
       <c r="E19" s="124"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="107"/>
+      <c r="F19" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="107">
+        <v>42684</v>
+      </c>
       <c r="I19" s="108"/>
       <c r="J19" s="97"/>
+    </row>
+    <row r="20" spans="1:10" ht="12" customHeight="1">
+      <c r="A20" s="124" t="str">
+        <f>IF(OR(B20&lt;&gt;"",D20&lt;E14&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-10]</v>
+      </c>
+      <c r="B20" s="105" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="105" t="s">
+        <v>157</v>
+      </c>
+      <c r="D20" s="105" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="124"/>
+      <c r="F20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I20" s="108"/>
+      <c r="J20" s="97"/>
+    </row>
+    <row r="21" spans="1:10" ht="12" customHeight="1">
+      <c r="A21" s="124" t="str">
+        <f>IF(OR(B21&lt;&gt;"",D21&lt;E15&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-11]</v>
+      </c>
+      <c r="B21" s="105" t="s">
+        <v>159</v>
+      </c>
+      <c r="C21" s="105" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" s="105" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" s="124"/>
+      <c r="F21" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I21" s="108"/>
+      <c r="J21" s="97"/>
+    </row>
+    <row r="22" spans="1:10" ht="12" customHeight="1">
+      <c r="A22" s="124" t="str">
+        <f t="shared" ref="A22:A27" si="1">IF(OR(B22&lt;&gt;"",D22&lt;E17&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-12]</v>
+      </c>
+      <c r="B22" s="105" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="105" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="105" t="s">
+        <v>178</v>
+      </c>
+      <c r="E22" s="124"/>
+      <c r="F22" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I22" s="108"/>
+      <c r="J22" s="97"/>
+    </row>
+    <row r="23" spans="1:10" ht="12" customHeight="1">
+      <c r="A23" s="124" t="str">
+        <f t="shared" si="1"/>
+        <v>[Common-13]</v>
+      </c>
+      <c r="B23" s="105" t="s">
+        <v>161</v>
+      </c>
+      <c r="C23" s="105" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="124"/>
+      <c r="F23" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I23" s="108"/>
+      <c r="J23" s="97"/>
+    </row>
+    <row r="24" spans="1:10" ht="12" customHeight="1">
+      <c r="A24" s="124" t="str">
+        <f t="shared" si="1"/>
+        <v>[Common-14]</v>
+      </c>
+      <c r="B24" s="105" t="s">
+        <v>162</v>
+      </c>
+      <c r="C24" s="105" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="105" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="124"/>
+      <c r="F24" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I24" s="108"/>
+      <c r="J24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" ht="12" customHeight="1">
+      <c r="A25" s="124" t="str">
+        <f t="shared" si="1"/>
+        <v>[Common-15]</v>
+      </c>
+      <c r="B25" s="105" t="s">
+        <v>163</v>
+      </c>
+      <c r="C25" s="105" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="105" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="124"/>
+      <c r="F25" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I25" s="108"/>
+      <c r="J25" s="97"/>
+    </row>
+    <row r="26" spans="1:10" ht="12" customHeight="1">
+      <c r="A26" s="124" t="str">
+        <f t="shared" si="1"/>
+        <v>[Common-16]</v>
+      </c>
+      <c r="B26" s="105" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="105" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" s="124"/>
+      <c r="F26" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I26" s="108"/>
+      <c r="J26" s="97"/>
+    </row>
+    <row r="27" spans="1:10" ht="12" customHeight="1">
+      <c r="A27" s="124" t="str">
+        <f t="shared" si="1"/>
+        <v>[Common-17]</v>
+      </c>
+      <c r="B27" s="105" t="s">
+        <v>165</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="105" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="124"/>
+      <c r="F27" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I27" s="108"/>
+      <c r="J27" s="97"/>
+    </row>
+    <row r="28" spans="1:10" ht="12" customHeight="1">
+      <c r="A28" s="124" t="str">
+        <f>IF(OR(B28&lt;&gt;"",D28&lt;E22&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-18]</v>
+      </c>
+      <c r="B28" s="105" t="s">
+        <v>166</v>
+      </c>
+      <c r="C28" s="105" t="s">
+        <v>169</v>
+      </c>
+      <c r="D28" s="105" t="s">
+        <v>179</v>
+      </c>
+      <c r="E28" s="124"/>
+      <c r="F28" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I28" s="108"/>
+      <c r="J28" s="97"/>
+    </row>
+    <row r="29" spans="1:10" ht="12" customHeight="1">
+      <c r="A29" s="124" t="str">
+        <f>IF(OR(B29&lt;&gt;"",D29&lt;E23&gt;""),"["&amp;TEXT($B$2,"##")&amp;"-"&amp;TEXT(ROW()-10,"##")&amp;"]","")</f>
+        <v>[Common-19]</v>
+      </c>
+      <c r="B29" s="105" t="s">
+        <v>167</v>
+      </c>
+      <c r="C29" s="105" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="105" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="124"/>
+      <c r="F29" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H29" s="107">
+        <v>42684</v>
+      </c>
+      <c r="I29" s="108"/>
+      <c r="J29" s="97"/>
     </row>
   </sheetData>
   <dataConsolidate>
@@ -6007,10 +6380,10 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G20:G65250">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G30:G65249">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12:G19">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F12:G29">
       <formula1>$J$2:$J$6</formula1>
     </dataValidation>
   </dataValidations>
@@ -6027,8 +6400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
@@ -6307,14 +6680,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="147" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="B2" s="149" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -6567,14 +6940,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="147" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
+      <c r="B3" s="149" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -6827,14 +7200,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="148" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
+      <c r="B4" s="150" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -7094,11 +7467,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -7350,26 +7723,26 @@
     <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="113">
         <f>COUNTIF(F11:G186,"Pass")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="94">
         <f>COUNTIF(F11:G633,"Fail")</f>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C6" s="94">
         <f>E6-D6-B6-A6</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D6" s="95">
-        <f>COUNTIF(F11:G633,"N/A")</f>
+        <f>COUNTIF(F11:G200,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="150">
-        <f>COUNTA(A11:A190)*2</f>
-        <v>24</v>
-      </c>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
+      <c r="E6" s="152">
+        <f>COUNTA(F12:F33)*2</f>
+        <v>28</v>
+      </c>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -8396,10 +8769,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>35</v>
@@ -8653,7 +9026,7 @@
     <row r="11" spans="1:257" s="88" customFormat="1" ht="14.25" customHeight="1">
       <c r="A11" s="127"/>
       <c r="B11" s="127" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C11" s="127"/>
       <c r="D11" s="127"/>
@@ -8663,24 +9036,30 @@
       <c r="H11" s="127"/>
       <c r="I11" s="132"/>
     </row>
-    <row r="12" spans="1:257" s="88" customFormat="1" ht="63.75" customHeight="1">
+    <row r="12" spans="1:257" s="88" customFormat="1" ht="65.25" customHeight="1">
       <c r="A12" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A11)+1)</f>
         <v>ID-2</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
+      <c r="F12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="107">
+        <v>42705</v>
+      </c>
       <c r="I12" s="105"/>
     </row>
     <row r="13" spans="1:257" s="88" customFormat="1" ht="51.75" customHeight="1">
@@ -8689,18 +9068,24 @@
         <v>ID-3</v>
       </c>
       <c r="B13" s="105" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
+      <c r="F13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="107">
+        <v>42705</v>
+      </c>
       <c r="I13" s="105"/>
     </row>
     <row r="14" spans="1:257" s="88" customFormat="1" ht="75" customHeight="1">
@@ -8709,35 +9094,47 @@
         <v>ID-4</v>
       </c>
       <c r="B14" s="135" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="C14" s="105" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
+      <c r="F14" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="107">
+        <v>42705</v>
+      </c>
       <c r="I14" s="105"/>
     </row>
     <row r="15" spans="1:257" s="88" customFormat="1" ht="75" customHeight="1">
       <c r="A15" s="105"/>
       <c r="B15" s="105" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
+      <c r="F15" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="107">
+        <v>42705</v>
+      </c>
       <c r="I15" s="105"/>
     </row>
     <row r="16" spans="1:257" s="88" customFormat="1" ht="72" customHeight="1">
@@ -8746,52 +9143,70 @@
         <v>ID-5</v>
       </c>
       <c r="B16" s="135" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
+      <c r="F16" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="107">
+        <v>42705</v>
+      </c>
       <c r="I16" s="105"/>
     </row>
     <row r="17" spans="1:10" s="88" customFormat="1" ht="72" customHeight="1">
       <c r="A17" s="105"/>
       <c r="B17" s="105" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
+      <c r="F17" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="107">
+        <v>42705</v>
+      </c>
       <c r="I17" s="105"/>
     </row>
     <row r="18" spans="1:10" s="88" customFormat="1" ht="72" customHeight="1">
       <c r="A18" s="105"/>
       <c r="B18" s="105" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
+      <c r="F18" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="107">
+        <v>42705</v>
+      </c>
       <c r="I18" s="105"/>
     </row>
     <row r="19" spans="1:10" s="88" customFormat="1" ht="70.5" customHeight="1">
@@ -8800,18 +9215,24 @@
         <v>ID-6</v>
       </c>
       <c r="B19" s="105" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
+      <c r="F19" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="107">
+        <v>42705</v>
+      </c>
       <c r="I19" s="105"/>
     </row>
     <row r="20" spans="1:10" s="88" customFormat="1" ht="70.5" customHeight="1">
@@ -8820,18 +9241,24 @@
         <v>ID-7</v>
       </c>
       <c r="B20" s="105" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="C20" s="105" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
+      <c r="F20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="107">
+        <v>42705</v>
+      </c>
       <c r="I20" s="105"/>
     </row>
     <row r="21" spans="1:10" s="88" customFormat="1" ht="67.5" customHeight="1">
@@ -8840,24 +9267,30 @@
         <v>ID-8</v>
       </c>
       <c r="B21" s="105" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="C21" s="105" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
+      <c r="F21" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="107">
+        <v>42705</v>
+      </c>
       <c r="I21" s="105"/>
     </row>
     <row r="22" spans="1:10" ht="12.75">
       <c r="A22" s="127"/>
       <c r="B22" s="127" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C22" s="127"/>
       <c r="D22" s="127"/>
@@ -8868,109 +9301,124 @@
       <c r="I22" s="131"/>
       <c r="J22" s="97"/>
     </row>
-    <row r="23" spans="1:10" ht="99" customHeight="1">
+    <row r="23" spans="1:10" ht="14.25" customHeight="1">
       <c r="A23" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A22)+1)</f>
         <v>ID-9</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C23" s="105" t="s">
-        <v>94</v>
+        <v>189</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
+      <c r="F23" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="107">
+        <v>42705</v>
+      </c>
       <c r="I23" s="105"/>
       <c r="J23" s="97"/>
     </row>
-    <row r="24" spans="1:10" ht="99" customHeight="1">
+    <row r="24" spans="1:10" ht="14.25" customHeight="1">
       <c r="A24" s="105" t="str">
+        <f>"ID-" &amp; (COUNTA(A$9:A22)+1)</f>
+        <v>ID-9</v>
+      </c>
+      <c r="B24" s="105" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="105" t="s">
+        <v>188</v>
+      </c>
+      <c r="D24" s="105" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="105"/>
+      <c r="F24" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="107">
+        <v>42705</v>
+      </c>
+      <c r="I24" s="105"/>
+      <c r="J24" s="97"/>
+    </row>
+    <row r="25" spans="1:10" ht="14.25" customHeight="1">
+      <c r="A25" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A23)+1)</f>
         <v>ID-10</v>
       </c>
-      <c r="B24" s="105" t="s">
-        <v>152</v>
-      </c>
-      <c r="C24" s="105" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="97"/>
-    </row>
-    <row r="25" spans="1:10" ht="114.75" customHeight="1">
-      <c r="A25" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A24)+1)</f>
-        <v>ID-11</v>
-      </c>
       <c r="B25" s="105" t="s">
-        <v>96</v>
+        <v>185</v>
       </c>
       <c r="C25" s="105" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
+      <c r="F25" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="107">
+        <v>42705</v>
+      </c>
       <c r="I25" s="105"/>
       <c r="J25" s="97"/>
     </row>
-    <row r="26" spans="1:10" ht="103.5" customHeight="1">
+    <row r="26" spans="1:10" ht="12.75" customHeight="1">
       <c r="A26" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A25)+1)</f>
         <v>ID-12</v>
       </c>
       <c r="B26" s="105" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="C26" s="105" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
+      <c r="F26" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="105" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="107">
+        <v>42705</v>
+      </c>
       <c r="I26" s="105"/>
       <c r="J26" s="97"/>
     </row>
-    <row r="27" spans="1:10" ht="114" customHeight="1">
-      <c r="A27" s="105" t="str">
-        <f>"ID-" &amp; (COUNTA(A$9:A26)+1)</f>
-        <v>ID-13</v>
-      </c>
-      <c r="B27" s="105" t="s">
-        <v>88</v>
-      </c>
-      <c r="C27" s="105" t="s">
-        <v>98</v>
-      </c>
-      <c r="D27" s="105" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
-      <c r="I27" s="105"/>
+    <row r="27" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A27" s="137"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
       <c r="J27" s="97"/>
     </row>
   </sheetData>
@@ -8987,13 +9435,13 @@
     <mergeCell ref="E6:G6"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IU12:JB21 SQ12:SX21 ACM12:ACT21 AMI12:AMP21 AWE12:AWL21 BGA12:BGH21 BPW12:BQD21 BZS12:BZZ21 CJO12:CJV21 CTK12:CTR21 DDG12:DDN21 DNC12:DNJ21 DWY12:DXF21 EGU12:EHB21 EQQ12:EQX21 FAM12:FAT21 FKI12:FKP21 FUE12:FUL21 GEA12:GEH21 GNW12:GOD21 GXS12:GXZ21 HHO12:HHV21 HRK12:HRR21 IBG12:IBN21 ILC12:ILJ21 IUY12:IVF21 JEU12:JFB21 JOQ12:JOX21 JYM12:JYT21 KII12:KIP21 KSE12:KSL21 LCA12:LCH21 LLW12:LMD21 LVS12:LVZ21 MFO12:MFV21 MPK12:MPR21 MZG12:MZN21 NJC12:NJJ21 NSY12:NTF21 OCU12:ODB21 OMQ12:OMX21 OWM12:OWT21 PGI12:PGP21 PQE12:PQL21 QAA12:QAH21 QJW12:QKD21 QTS12:QTZ21 RDO12:RDV21 RNK12:RNR21 RXG12:RXN21 SHC12:SHJ21 SQY12:SRF21 TAU12:TBB21 TKQ12:TKX21 TUM12:TUT21 UEI12:UEP21 UOE12:UOL21 UYA12:UYH21 VHW12:VID21 VRS12:VRZ21 WBO12:WBV21 WLK12:WLR21 WVG12:WVN21 WLU11:WLU26 VSC11:VSC26 WVQ11:WVQ26 WBY11:WBY26 WVG23:WVN26 WLK23:WLR26 WBO23:WBV26 VRS23:VRZ26 VHW23:VID26 UYA23:UYH26 UOE23:UOL26 UEI23:UEP26 TUM23:TUT26 TKQ23:TKX26 TAU23:TBB26 SQY23:SRF26 SHC23:SHJ26 RXG23:RXN26 RNK23:RNR26 RDO23:RDV26 QTS23:QTZ26 QJW23:QKD26 QAA23:QAH26 PQE23:PQL26 PGI23:PGP26 OWM23:OWT26 OMQ23:OMX26 OCU23:ODB26 NSY23:NTF26 NJC23:NJJ26 MZG23:MZN26 MPK23:MPR26 MFO23:MFV26 LVS23:LVZ26 LLW23:LMD26 LCA23:LCH26 KSE23:KSL26 KII23:KIP26 JYM23:JYT26 JOQ23:JOX26 JEU23:JFB26 IUY23:IVF26 ILC23:ILJ26 IBG23:IBN26 HRK23:HRR26 HHO23:HHV26 GXS23:GXZ26 GNW23:GOD26 GEA23:GEH26 FUE23:FUL26 FKI23:FKP26 FAM23:FAT26 EQQ23:EQX26 EGU23:EHB26 DWY23:DXF26 DNC23:DNJ26 DDG23:DDN26 CTK23:CTR26 CJO23:CJV26 BZS23:BZZ26 BPW23:BQD26 BGA23:BGH26 AWE23:AWL26 AMI23:AMP26 ACM23:ACT26 SQ23:SX26 IU23:JB26 JE11:JE26 TA11:TA26 ACW11:ACW26 AMS11:AMS26 AWO11:AWO26 BGK11:BGK26 BQG11:BQG26 CAC11:CAC26 CJY11:CJY26 CTU11:CTU26 DDQ11:DDQ26 DNM11:DNM26 DXI11:DXI26 EHE11:EHE26 ERA11:ERA26 FAW11:FAW26 FKS11:FKS26 FUO11:FUO26 GEK11:GEK26 GOG11:GOG26 GYC11:GYC26 HHY11:HHY26 HRU11:HRU26 IBQ11:IBQ26 ILM11:ILM26 IVI11:IVI26 JFE11:JFE26 JPA11:JPA26 JYW11:JYW26 KIS11:KIS26 KSO11:KSO26 LCK11:LCK26 LMG11:LMG26 LWC11:LWC26 MFY11:MFY26 MPU11:MPU26 MZQ11:MZQ26 NJM11:NJM26 NTI11:NTI26 ODE11:ODE26 ONA11:ONA26 OWW11:OWW26 PGS11:PGS26 PQO11:PQO26 QAK11:QAK26 QKG11:QKG26 QUC11:QUC26 RDY11:RDY26 RNU11:RNU26 RXQ11:RXQ26 SHM11:SHM26 SRI11:SRI26 TBE11:TBE26 TLA11:TLA26 TUW11:TUW26 UES11:UES26 UOO11:UOO26 UYK11:UYK26 VIG11:VIG26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="IU12:JB21 SQ12:SX21 ACM12:ACT21 AMI12:AMP21 AWE12:AWL21 BGA12:BGH21 BPW12:BQD21 BZS12:BZZ21 CJO12:CJV21 CTK12:CTR21 DDG12:DDN21 DNC12:DNJ21 DWY12:DXF21 EGU12:EHB21 EQQ12:EQX21 FAM12:FAT21 FKI12:FKP21 FUE12:FUL21 GEA12:GEH21 GNW12:GOD21 GXS12:GXZ21 HHO12:HHV21 HRK12:HRR21 IBG12:IBN21 ILC12:ILJ21 IUY12:IVF21 JEU12:JFB21 JOQ12:JOX21 JYM12:JYT21 KII12:KIP21 KSE12:KSL21 LCA12:LCH21 LLW12:LMD21 LVS12:LVZ21 MFO12:MFV21 MPK12:MPR21 MZG12:MZN21 NJC12:NJJ21 NSY12:NTF21 OCU12:ODB21 OMQ12:OMX21 OWM12:OWT21 PGI12:PGP21 PQE12:PQL21 QAA12:QAH21 QJW12:QKD21 QTS12:QTZ21 RDO12:RDV21 RNK12:RNR21 RXG12:RXN21 SHC12:SHJ21 SQY12:SRF21 TAU12:TBB21 TKQ12:TKX21 TUM12:TUT21 UEI12:UEP21 UOE12:UOL21 UYA12:UYH21 VHW12:VID21 VRS12:VRZ21 WBO12:WBV21 WLK12:WLR21 WVG12:WVN21 VIG11:VIG27 UYK11:UYK27 UOO11:UOO27 UES11:UES27 TUW11:TUW27 TLA11:TLA27 TBE11:TBE27 SRI11:SRI27 SHM11:SHM27 RXQ11:RXQ27 RNU11:RNU27 RDY11:RDY27 QUC11:QUC27 QKG11:QKG27 QAK11:QAK27 PQO11:PQO27 PGS11:PGS27 OWW11:OWW27 ONA11:ONA27 ODE11:ODE27 NTI11:NTI27 NJM11:NJM27 MZQ11:MZQ27 MPU11:MPU27 MFY11:MFY27 LWC11:LWC27 LMG11:LMG27 LCK11:LCK27 KSO11:KSO27 KIS11:KIS27 JYW11:JYW27 JPA11:JPA27 JFE11:JFE27 IVI11:IVI27 ILM11:ILM27 IBQ11:IBQ27 HRU11:HRU27 HHY11:HHY27 GYC11:GYC27 GOG11:GOG27 GEK11:GEK27 FUO11:FUO27 FKS11:FKS27 FAW11:FAW27 ERA11:ERA27 EHE11:EHE27 DXI11:DXI27 DNM11:DNM27 DDQ11:DDQ27 CTU11:CTU27 CJY11:CJY27 CAC11:CAC27 BQG11:BQG27 BGK11:BGK27 AWO11:AWO27 AMS11:AMS27 ACW11:ACW27 TA11:TA27 JE11:JE27 IU23:JB27 SQ23:SX27 ACM23:ACT27 AMI23:AMP27 AWE23:AWL27 BGA23:BGH27 BPW23:BQD27 BZS23:BZZ27 CJO23:CJV27 CTK23:CTR27 DDG23:DDN27 DNC23:DNJ27 DWY23:DXF27 EGU23:EHB27 EQQ23:EQX27 FAM23:FAT27 FKI23:FKP27 FUE23:FUL27 GEA23:GEH27 GNW23:GOD27 GXS23:GXZ27 HHO23:HHV27 HRK23:HRR27 IBG23:IBN27 ILC23:ILJ27 IUY23:IVF27 JEU23:JFB27 JOQ23:JOX27 JYM23:JYT27 KII23:KIP27 KSE23:KSL27 LCA23:LCH27 LLW23:LMD27 LVS23:LVZ27 MFO23:MFV27 MPK23:MPR27 MZG23:MZN27 NJC23:NJJ27 NSY23:NTF27 OCU23:ODB27 OMQ23:OMX27 OWM23:OWT27 PGI23:PGP27 PQE23:PQL27 QAA23:QAH27 QJW23:QKD27 QTS23:QTZ27 RDO23:RDV27 RNK23:RNR27 RXG23:RXN27 SHC23:SHJ27 SQY23:SRF27 TAU23:TBB27 TKQ23:TKX27 TUM23:TUT27 UEI23:UEP27 UOE23:UOL27 UYA23:UYH27 VHW23:VID27 VRS23:VRZ27 WBO23:WBV27 WLK23:WLR27 WVG23:WVN27 WBY11:WBY27 WVQ11:WVQ27 VSC11:VSC27 WLU11:WLU27">
       <formula1>"OK,NG,N/A"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G28:G65258">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F23:G27 F12:G21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F12:G21 F23:G27">
       <formula1>$A$5:$D$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -9010,7 +9458,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IW27"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.25" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
@@ -9288,14 +9738,14 @@
       <c r="A2" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="147" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="B2" s="149" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="149"/>
+      <c r="D2" s="149"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
       <c r="H2" s="117" t="s">
         <v>22</v>
       </c>
@@ -9548,14 +9998,14 @@
       <c r="A3" s="111" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="147" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="147"/>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="147"/>
+      <c r="B3" s="149" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="149"/>
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="117" t="s">
         <v>24</v>
       </c>
@@ -9808,14 +10258,14 @@
       <c r="A4" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="148" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
+      <c r="B4" s="150" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="150"/>
+      <c r="D4" s="150"/>
+      <c r="E4" s="150"/>
+      <c r="F4" s="150"/>
+      <c r="G4" s="150"/>
       <c r="H4" s="117" t="s">
         <v>27</v>
       </c>
@@ -10075,11 +10525,11 @@
       <c r="D5" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="149" t="s">
+      <c r="E5" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
+      <c r="F5" s="151"/>
+      <c r="G5" s="151"/>
       <c r="H5" s="118" t="s">
         <v>26</v>
       </c>
@@ -10331,7 +10781,7 @@
     <row r="6" spans="1:257" ht="13.5" customHeight="1" thickBot="1">
       <c r="A6" s="113">
         <f>COUNTIF(F11:G186,"Pass")</f>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B6" s="94">
         <f>COUNTIF(F11:G633,"Fail")</f>
@@ -10339,18 +10789,18 @@
       </c>
       <c r="C6" s="94">
         <f>E6-D6-B6-A6</f>
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D6" s="95">
         <f>COUNTIF(F11:G633,"N/A")</f>
         <v>0</v>
       </c>
-      <c r="E6" s="150">
+      <c r="E6" s="152">
         <f>COUNTA(A11:A190)*2</f>
         <v>32</v>
       </c>
-      <c r="F6" s="150"/>
-      <c r="G6" s="150"/>
+      <c r="F6" s="152"/>
+      <c r="G6" s="152"/>
       <c r="H6" s="92"/>
       <c r="I6" s="88"/>
       <c r="J6" s="88" t="s">
@@ -11377,10 +11827,10 @@
         <v>34</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="H10" s="57" t="s">
         <v>35</v>
@@ -11633,7 +12083,7 @@
     <row r="11" spans="1:257" s="88" customFormat="1" ht="12.75">
       <c r="A11" s="127"/>
       <c r="B11" s="127" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="127"/>
       <c r="D11" s="127"/>
@@ -11649,18 +12099,24 @@
         <v>ID-2</v>
       </c>
       <c r="B12" s="105" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C12" s="105" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="133" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="E12" s="105"/>
-      <c r="F12" s="105"/>
-      <c r="G12" s="105"/>
-      <c r="H12" s="105"/>
+      <c r="F12" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="107">
+        <v>42684</v>
+      </c>
       <c r="I12" s="105"/>
     </row>
     <row r="13" spans="1:257" s="88" customFormat="1" ht="36" customHeight="1">
@@ -11669,18 +12125,24 @@
         <v>ID-2</v>
       </c>
       <c r="B13" s="105" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C13" s="105" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
+      <c r="F13" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="107">
+        <v>42684</v>
+      </c>
       <c r="I13" s="105"/>
     </row>
     <row r="14" spans="1:257" s="88" customFormat="1" ht="36" customHeight="1">
@@ -11689,18 +12151,24 @@
         <v>ID-3</v>
       </c>
       <c r="B14" s="105" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="C14" s="105" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="E14" s="105"/>
-      <c r="F14" s="105"/>
-      <c r="G14" s="105"/>
-      <c r="H14" s="105"/>
+      <c r="F14" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="107">
+        <v>42684</v>
+      </c>
       <c r="I14" s="105"/>
     </row>
     <row r="15" spans="1:257" s="88" customFormat="1" ht="25.5">
@@ -11709,18 +12177,24 @@
         <v>ID-4</v>
       </c>
       <c r="B15" s="105" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C15" s="105" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E15" s="105"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="105"/>
-      <c r="H15" s="105"/>
+      <c r="F15" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="107">
+        <v>42684</v>
+      </c>
       <c r="I15" s="105"/>
     </row>
     <row r="16" spans="1:257" s="88" customFormat="1" ht="25.5">
@@ -11729,18 +12203,24 @@
         <v>ID-5</v>
       </c>
       <c r="B16" s="105" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="E16" s="105"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="105"/>
-      <c r="H16" s="105"/>
+      <c r="F16" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="107">
+        <v>42684</v>
+      </c>
       <c r="I16" s="105"/>
     </row>
     <row r="17" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11749,18 +12229,24 @@
         <v>ID-6</v>
       </c>
       <c r="B17" s="105" t="s">
-        <v>60</v>
+        <v>181</v>
       </c>
       <c r="C17" s="105" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E17" s="105"/>
-      <c r="F17" s="105"/>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
+      <c r="F17" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="107">
+        <v>42684</v>
+      </c>
       <c r="I17" s="105"/>
     </row>
     <row r="18" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11769,18 +12255,24 @@
         <v>ID-8</v>
       </c>
       <c r="B18" s="105" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C18" s="105" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E18" s="105"/>
-      <c r="F18" s="105"/>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
+      <c r="F18" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="107">
+        <v>42684</v>
+      </c>
       <c r="I18" s="105"/>
     </row>
     <row r="19" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11789,18 +12281,24 @@
         <v>ID-9</v>
       </c>
       <c r="B19" s="105" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C19" s="105" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="E19" s="105"/>
-      <c r="F19" s="105"/>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
+      <c r="F19" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="107">
+        <v>42684</v>
+      </c>
       <c r="I19" s="105"/>
     </row>
     <row r="20" spans="1:9" s="88" customFormat="1" ht="40.5" customHeight="1">
@@ -11809,18 +12307,24 @@
         <v>ID-10</v>
       </c>
       <c r="B20" s="105" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" s="105" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E20" s="105"/>
-      <c r="F20" s="105"/>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
+      <c r="F20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="107">
+        <v>42684</v>
+      </c>
       <c r="I20" s="105"/>
     </row>
     <row r="21" spans="1:9" s="88" customFormat="1" ht="43.5" customHeight="1">
@@ -11829,18 +12333,24 @@
         <v>ID-11</v>
       </c>
       <c r="B21" s="105" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" s="105" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E21" s="105"/>
-      <c r="F21" s="105"/>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
+      <c r="F21" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="107">
+        <v>42684</v>
+      </c>
       <c r="I21" s="105"/>
     </row>
     <row r="22" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11849,18 +12359,24 @@
         <v>ID-12</v>
       </c>
       <c r="B22" s="105" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C22" s="105" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" s="105" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E22" s="105"/>
-      <c r="F22" s="105"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="105"/>
+      <c r="F22" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="107">
+        <v>42684</v>
+      </c>
       <c r="I22" s="105"/>
     </row>
     <row r="23" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11869,38 +12385,50 @@
         <v>ID-13</v>
       </c>
       <c r="B23" s="105" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C23" s="105" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="105"/>
+      <c r="F23" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="107">
+        <v>42684</v>
+      </c>
       <c r="I23" s="105"/>
     </row>
-    <row r="24" spans="1:9" s="88" customFormat="1" ht="12.75">
+    <row r="24" spans="1:9" s="88" customFormat="1" ht="25.5">
       <c r="A24" s="105" t="str">
         <f>"ID-" &amp; (COUNTA(A$9:A23)+1)</f>
         <v>ID-14</v>
       </c>
       <c r="B24" s="105" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24" s="105" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
-      <c r="G24" s="105"/>
-      <c r="H24" s="105"/>
+      <c r="F24" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="107">
+        <v>42684</v>
+      </c>
       <c r="I24" s="105"/>
     </row>
     <row r="25" spans="1:9" s="88" customFormat="1" ht="12.75">
@@ -11909,18 +12437,24 @@
         <v>ID-15</v>
       </c>
       <c r="B25" s="105" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C25" s="105" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E25" s="105"/>
-      <c r="F25" s="105"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
+      <c r="F25" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="107">
+        <v>42684</v>
+      </c>
       <c r="I25" s="105"/>
     </row>
     <row r="26" spans="1:9" s="88" customFormat="1" ht="12.75">
@@ -11929,18 +12463,24 @@
         <v>ID-16</v>
       </c>
       <c r="B26" s="105" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="C26" s="105" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="E26" s="105"/>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105"/>
+      <c r="F26" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="107">
+        <v>42684</v>
+      </c>
       <c r="I26" s="105"/>
     </row>
     <row r="27" spans="1:9" s="88" customFormat="1" ht="25.5">
@@ -11949,18 +12489,24 @@
         <v>ID-17</v>
       </c>
       <c r="B27" s="105" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C27" s="105" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D27" s="105" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
-      <c r="H27" s="105"/>
+      <c r="F27" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="105" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="107">
+        <v>42684</v>
+      </c>
       <c r="I27" s="105"/>
     </row>
   </sheetData>
@@ -11980,7 +12526,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G9 G28:G65258">
       <formula1>$H$2:$H$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WLJ12:WLQ27 F12:G27 SZ11:SZ27 ACV11:ACV27 AMR11:AMR27 AWN11:AWN27 BGJ11:BGJ27 BQF11:BQF27 CAB11:CAB27 CJX11:CJX27 CTT11:CTT27 DDP11:DDP27 DNL11:DNL27 DXH11:DXH27 EHD11:EHD27 EQZ11:EQZ27 FAV11:FAV27 FKR11:FKR27 FUN11:FUN27 GEJ11:GEJ27 GOF11:GOF27 GYB11:GYB27 HHX11:HHX27 HRT11:HRT27 IBP11:IBP27 ILL11:ILL27 IVH11:IVH27 JFD11:JFD27 JOZ11:JOZ27 JYV11:JYV27 KIR11:KIR27 KSN11:KSN27 LCJ11:LCJ27 LMF11:LMF27 LWB11:LWB27 MFX11:MFX27 MPT11:MPT27 MZP11:MZP27 NJL11:NJL27 NTH11:NTH27 ODD11:ODD27 OMZ11:OMZ27 OWV11:OWV27 PGR11:PGR27 PQN11:PQN27 QAJ11:QAJ27 QKF11:QKF27 QUB11:QUB27 RDX11:RDX27 RNT11:RNT27 RXP11:RXP27 SHL11:SHL27 SRH11:SRH27 TBD11:TBD27 TKZ11:TKZ27 TUV11:TUV27 UER11:UER27 UON11:UON27 UYJ11:UYJ27 VIF11:VIF27 VSB11:VSB27 WBX11:WBX27 WLT11:WLT27 WVP11:WVP27 WVF12:WVM27 JD11:JD27 IT12:JA27 SP12:SW27 ACL12:ACS27 AMH12:AMO27 AWD12:AWK27 BFZ12:BGG27 BPV12:BQC27 BZR12:BZY27 CJN12:CJU27 CTJ12:CTQ27 DDF12:DDM27 DNB12:DNI27 DWX12:DXE27 EGT12:EHA27 EQP12:EQW27 FAL12:FAS27 FKH12:FKO27 FUD12:FUK27 GDZ12:GEG27 GNV12:GOC27 GXR12:GXY27 HHN12:HHU27 HRJ12:HRQ27 IBF12:IBM27 ILB12:ILI27 IUX12:IVE27 JET12:JFA27 JOP12:JOW27 JYL12:JYS27 KIH12:KIO27 KSD12:KSK27 LBZ12:LCG27 LLV12:LMC27 LVR12:LVY27 MFN12:MFU27 MPJ12:MPQ27 MZF12:MZM27 NJB12:NJI27 NSX12:NTE27 OCT12:ODA27 OMP12:OMW27 OWL12:OWS27 PGH12:PGO27 PQD12:PQK27 PZZ12:QAG27 QJV12:QKC27 QTR12:QTY27 RDN12:RDU27 RNJ12:RNQ27 RXF12:RXM27 SHB12:SHI27 SQX12:SRE27 TAT12:TBA27 TKP12:TKW27 TUL12:TUS27 UEH12:UEO27 UOD12:UOK27 UXZ12:UYG27 VHV12:VIC27 VRR12:VRY27 WBN12:WBU27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="WLJ12:WLQ27 WBN12:WBU27 SZ11:SZ27 ACV11:ACV27 AMR11:AMR27 AWN11:AWN27 BGJ11:BGJ27 BQF11:BQF27 CAB11:CAB27 CJX11:CJX27 CTT11:CTT27 DDP11:DDP27 DNL11:DNL27 DXH11:DXH27 EHD11:EHD27 EQZ11:EQZ27 FAV11:FAV27 FKR11:FKR27 FUN11:FUN27 GEJ11:GEJ27 GOF11:GOF27 GYB11:GYB27 HHX11:HHX27 HRT11:HRT27 IBP11:IBP27 ILL11:ILL27 IVH11:IVH27 JFD11:JFD27 JOZ11:JOZ27 JYV11:JYV27 KIR11:KIR27 KSN11:KSN27 LCJ11:LCJ27 LMF11:LMF27 LWB11:LWB27 MFX11:MFX27 MPT11:MPT27 MZP11:MZP27 NJL11:NJL27 NTH11:NTH27 ODD11:ODD27 OMZ11:OMZ27 OWV11:OWV27 PGR11:PGR27 PQN11:PQN27 QAJ11:QAJ27 QKF11:QKF27 QUB11:QUB27 RDX11:RDX27 RNT11:RNT27 RXP11:RXP27 SHL11:SHL27 SRH11:SRH27 TBD11:TBD27 TKZ11:TKZ27 TUV11:TUV27 UER11:UER27 UON11:UON27 UYJ11:UYJ27 VIF11:VIF27 VSB11:VSB27 WBX11:WBX27 WLT11:WLT27 WVP11:WVP27 WVF12:WVM27 JD11:JD27 IT12:JA27 SP12:SW27 ACL12:ACS27 AMH12:AMO27 AWD12:AWK27 BFZ12:BGG27 BPV12:BQC27 BZR12:BZY27 CJN12:CJU27 CTJ12:CTQ27 DDF12:DDM27 DNB12:DNI27 DWX12:DXE27 EGT12:EHA27 EQP12:EQW27 FAL12:FAS27 FKH12:FKO27 FUD12:FUK27 GDZ12:GEG27 GNV12:GOC27 GXR12:GXY27 HHN12:HHU27 HRJ12:HRQ27 IBF12:IBM27 ILB12:ILI27 IUX12:IVE27 JET12:JFA27 JOP12:JOW27 JYL12:JYS27 KIH12:KIO27 KSD12:KSK27 LBZ12:LCG27 LLV12:LMC27 LVR12:LVY27 MFN12:MFU27 MPJ12:MPQ27 MZF12:MZM27 NJB12:NJI27 NSX12:NTE27 OCT12:ODA27 OMP12:OMW27 OWL12:OWS27 PGH12:PGO27 PQD12:PQK27 PZZ12:QAG27 QJV12:QKC27 QTR12:QTY27 RDN12:RDU27 RNJ12:RNQ27 RXF12:RXM27 SHB12:SHI27 SQX12:SRE27 TAT12:TBA27 TKP12:TKW27 TUL12:TUS27 UEH12:UEO27 UOD12:UOK27 UXZ12:UYG27 VHV12:VIC27 VRR12:VRY27 F12:G27">
       <formula1>$J$2:$J$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>